<commit_message>
Working framework completed.. Code cleanup required..
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
   <si>
     <t>Name</t>
   </si>
@@ -132,9 +132,6 @@
     <t>http://www.sha1-online.com/</t>
   </si>
   <si>
-    <t>https://acme-test.uipath.com/account/login</t>
-  </si>
-  <si>
     <t>Credential name for System1. The value must match with credentials name defined in Orchestrator.</t>
   </si>
   <si>
@@ -142,6 +139,15 @@
   </si>
   <si>
     <t>URL for SHA1 online web applcation.</t>
+  </si>
+  <si>
+    <t>https://acme-test.uipath.com/</t>
+  </si>
+  <si>
+    <t>TimeoutShort</t>
+  </si>
+  <si>
+    <t>Timeout for activities like element exist</t>
   </si>
 </sst>
 </file>
@@ -520,7 +526,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -594,10 +600,10 @@
         <v>31</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
@@ -608,7 +614,7 @@
         <v>34</v>
       </c>
       <c r="C7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
@@ -620,7 +626,7 @@
         <v>33</v>
       </c>
       <c r="C9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1623,7 +1629,7 @@
   <dimension ref="A1:Z987"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1748,7 +1754,17 @@
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12">
+        <v>5000</v>
+      </c>
+      <c r="C12" t="s">
+        <v>40</v>
+      </c>
+    </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Value changed for slower data connection
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\793122\Documents\UiPath\Generate_Yearly_Report\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tehri\Documents\UiPath\Generate_Yearly_Report\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{038A6CAB-F481-4987-8F7B-ACEF103752C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -143,7 +144,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -512,19 +513,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z996"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5703125" customWidth="1"/>
+    <col min="1" max="1" width="43.5546875" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="81.44140625" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -573,7 +574,7 @@
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="4" spans="1:26" ht="30">
+    <row r="4" spans="1:26" ht="28.8">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -1604,19 +1605,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="75.44140625" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1653,7 +1654,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="30">
+    <row r="2" spans="1:26" ht="28.8">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1738,7 +1739,7 @@
         <v>34</v>
       </c>
       <c r="B12">
-        <v>2000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
@@ -2730,17 +2731,17 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1"/>
-    <col min="2" max="2" width="30.140625" customWidth="1"/>
-    <col min="3" max="3" width="60.28515625" customWidth="1"/>
-    <col min="4" max="26" width="65.42578125" customWidth="1"/>
+    <col min="1" max="1" width="31.88671875" customWidth="1"/>
+    <col min="2" max="2" width="30.109375" customWidth="1"/>
+    <col min="3" max="3" width="60.33203125" customWidth="1"/>
+    <col min="4" max="26" width="65.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>